<commit_message>
Made some progress on converting the ica data.
</commit_message>
<xml_diff>
--- a/Examensarbete.xlsx
+++ b/Examensarbete.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08f85b3e17695a97/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\examensarbete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{4F0413CC-FEA5-49AE-980B-01515B52080D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E02653DA-DAAD-4C07-9438-DF4A04C06BC8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA461BEF-2548-4C4A-8133-3BB76E58B492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{05FF577A-4931-4F6F-86DB-9A3320FD4ACE}"/>
+    <workbookView xWindow="30795" yWindow="6180" windowWidth="17730" windowHeight="10140" activeTab="1" xr2:uid="{05FF577A-4931-4F6F-86DB-9A3320FD4ACE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ica-Api" sheetId="4" r:id="rId2"/>
-    <sheet name="Willys-Api" sheetId="5" r:id="rId3"/>
-    <sheet name="Endpoints" sheetId="3" r:id="rId4"/>
-    <sheet name="Databas" sheetId="2" r:id="rId5"/>
+    <sheet name="Frontend" sheetId="6" r:id="rId2"/>
+    <sheet name="Ica-Api" sheetId="4" r:id="rId3"/>
+    <sheet name="Willys-Api" sheetId="5" r:id="rId4"/>
+    <sheet name="Endpoints" sheetId="3" r:id="rId5"/>
+    <sheet name="Databas" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Recept-community</t>
   </si>
@@ -136,6 +137,15 @@
   </si>
   <si>
     <t>Alingsås</t>
+  </si>
+  <si>
+    <t>React mobile web first</t>
+  </si>
+  <si>
+    <t>Pwa för att undvika appstore</t>
+  </si>
+  <si>
+    <t>Progressive web app</t>
   </si>
 </sst>
 </file>
@@ -190,14 +200,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,7 +241,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -341,7 +347,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -483,7 +489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,7 +500,7 @@
   <dimension ref="C2:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,6 +545,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D09D594-A0E5-4690-B20F-066DA5210658}">
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6690303F-3627-420A-8CAF-929B8D6EED7B}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -550,11 +586,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41067001-B98D-4E2B-885D-32C229936B35}">
   <dimension ref="B3:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -592,7 +628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AC0AFC-B1F2-46CF-97E2-C131EEB345BD}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -606,7 +642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA782E68-E829-4ED2-B006-AD8AE90B769A}">
   <dimension ref="C2:M9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Testing to read in ingredients from livsmedelsverket.
</commit_message>
<xml_diff>
--- a/Examensarbete.xlsx
+++ b/Examensarbete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\examensarbete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA461BEF-2548-4C4A-8133-3BB76E58B492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AB82E5-E67C-4CBF-B45F-CC1DC661FCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30795" yWindow="6180" windowWidth="17730" windowHeight="10140" activeTab="1" xr2:uid="{05FF577A-4931-4F6F-86DB-9A3320FD4ACE}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="30570" windowHeight="20985" activeTab="5" xr2:uid="{05FF577A-4931-4F6F-86DB-9A3320FD4ACE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Willys-Api" sheetId="5" r:id="rId4"/>
     <sheet name="Endpoints" sheetId="3" r:id="rId5"/>
     <sheet name="Databas" sheetId="2" r:id="rId6"/>
+    <sheet name="TestRecept" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Recept-community</t>
   </si>
@@ -109,9 +110,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>list of ingridents</t>
-  </si>
-  <si>
     <t>instructions</t>
   </si>
   <si>
@@ -146,6 +144,52 @@
   </si>
   <si>
     <t>Progressive web app</t>
+  </si>
+  <si>
+    <t>Checklista innan handling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Möjlighet att kunna få en checklista på de varor man har I skafferiet osv. </t>
+  </si>
+  <si>
+    <t>difficulty</t>
+  </si>
+  <si>
+    <t>portions</t>
+  </si>
+  <si>
+    <t>subRecipe</t>
+  </si>
+  <si>
+    <t>subrecipes</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>NumberOfPortions</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Time h</t>
+  </si>
+  <si>
+    <t>Färgglad pastasallad med fläskfile</t>
+  </si>
+  <si>
+    <t>Putsa köttet från senor och hinnor. Skär det i 2 cm tjocka bitar. Blanda vetemjöl, salt och peppar och vänd köttet i det.
+Bryn köttet på båda sidor i en medelvarm panna. Stek dem därefter 2-3 minuter tills köttet är genomstekt. 
+Koka pastan enligt anvisning på paketet, men utan salt, eftersom rätten i övrigt ger så mycket smak. Låt sockerärter eller haricotsverts koka med sista 2-3 minuterna. Häll av i durkslag och skölj med kallt vatten. 
+Riv morötterna. Skär gurkan i tärningar och tomaterna i bitar. Blanda alla grönsaker med pastan.
+Blanda dressingen och häll över. Fördela köttet över salladen och servera med bröd.</t>
+  </si>
+  <si>
+    <t>Image link</t>
   </si>
 </sst>
 </file>
@@ -181,13 +225,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -198,6 +249,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DA3EEA8-3AB9-4518-AF59-DD1FCF2C0278}" name="Table1" displayName="Table1" ref="F1:K2" totalsRowShown="0">
+  <autoFilter ref="F1:K2" xr:uid="{7DA3EEA8-3AB9-4518-AF59-DD1FCF2C0278}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{660F27E7-87F6-42A9-A0F6-01D6148AFC79}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{2A96AF1D-0018-4212-A74C-CAF859624AEE}" name="Time h"/>
+    <tableColumn id="3" xr3:uid="{5C8280AC-CA8D-438D-A2FA-33AFA05D6869}" name="NumberOfPortions"/>
+    <tableColumn id="4" xr3:uid="{22E927FE-3F8F-40AF-96BD-E79A27ABCABA}" name="Difficulty"/>
+    <tableColumn id="5" xr3:uid="{CF491F4D-7CC9-4A51-B7BC-294AB372DE36}" name="Instructions" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{6A444BC6-4431-4749-9C06-0026181A8D05}" name="Image link"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,12 +566,12 @@
   <dimension ref="C2:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
@@ -524,6 +590,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
@@ -531,12 +605,12 @@
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -548,7 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D09D594-A0E5-4690-B20F-066DA5210658}">
   <dimension ref="A2:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -556,17 +630,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -601,15 +675,15 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>2103</v>
@@ -617,7 +691,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>2149</v>
@@ -644,15 +718,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA782E68-E829-4ED2-B006-AD8AE90B769A}">
-  <dimension ref="C2:M9"/>
+  <dimension ref="C2:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -666,13 +740,16 @@
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -685,14 +762,14 @@
       <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>7</v>
       </c>
@@ -703,13 +780,13 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -720,33 +797,141 @@
         <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92CDF48-A787-4E9F-813D-0D0B461723F4}">
+  <dimension ref="C1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="3:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>